<commit_message>
updated timelog with Filips data
</commit_message>
<xml_diff>
--- a/references/Timelog.xlsx
+++ b/references/Timelog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenna\Documents\GoogleDrive\Studium\DoDWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fleip/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65389367-70E4-45A9-9051-B964279762FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A0814A-2FB6-7140-826C-3A25D437C7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71DC7254-18A5-40D2-832D-9A5408E948A6}"/>
+    <workbookView xWindow="-2700" yWindow="-42700" windowWidth="76800" windowHeight="42700" xr2:uid="{71DC7254-18A5-40D2-832D-9A5408E948A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -90,13 +90,13 @@
     <t>Week 2</t>
   </si>
   <si>
-    <t>Coordination</t>
-  </si>
-  <si>
     <t>Security</t>
   </si>
   <si>
     <t>Documentation</t>
+  </si>
+  <si>
+    <t>Team Meetings</t>
   </si>
 </sst>
 </file>
@@ -211,18 +211,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -232,9 +226,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -250,7 +251,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -548,381 +549,431 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23DFFBD-25A4-4452-A7FA-D1CCCE610C36}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="10"/>
-    <col min="3" max="3" width="11.5546875" style="14"/>
-    <col min="6" max="6" width="11.5546875" style="10"/>
-    <col min="7" max="7" width="11.5546875" style="14"/>
-    <col min="10" max="10" width="11.5546875" style="10"/>
-    <col min="11" max="11" width="11.5546875" style="14"/>
-    <col min="14" max="14" width="11.5546875" style="10"/>
-    <col min="15" max="15" width="11.5546875" style="14"/>
-    <col min="18" max="18" width="11.5546875" style="10"/>
-    <col min="19" max="19" width="11.5546875" style="14"/>
-    <col min="22" max="22" width="11.5546875" style="10"/>
-    <col min="23" max="23" width="11.5546875" style="14"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="8"/>
+    <col min="3" max="3" width="11.5" style="12"/>
+    <col min="6" max="6" width="11.5" style="8"/>
+    <col min="7" max="7" width="11.5" style="12"/>
+    <col min="10" max="10" width="11.5" style="8"/>
+    <col min="11" max="11" width="11.5" style="12"/>
+    <col min="14" max="14" width="11.5" style="8"/>
+    <col min="15" max="15" width="11.5" style="12"/>
+    <col min="18" max="18" width="11.5" style="8"/>
+    <col min="19" max="19" width="11.5" style="12"/>
+    <col min="22" max="22" width="11.5" style="8"/>
+    <col min="23" max="23" width="11.5" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6" t="s">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6" t="s">
+      <c r="S1" s="14"/>
+      <c r="T1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6" t="s">
+      <c r="U1" s="14"/>
+      <c r="V1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="6"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
     </row>
-    <row r="2" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" s="7" t="s">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>6</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="5">
-        <v>4</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="12"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="12"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="12"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="12"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="12"/>
+      <c r="C3" s="10">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="10"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="10"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="10"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="10"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="11">
+        <v>2</v>
+      </c>
       <c r="D4" s="1">
         <v>7</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="13"/>
+      <c r="E4" s="1">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="9">
+      <c r="I4" s="16">
+        <v>2</v>
+      </c>
+      <c r="J4" s="7">
         <v>6</v>
       </c>
-      <c r="K4" s="13"/>
+      <c r="K4" s="11">
+        <v>2</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="13"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="11"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="13"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="11"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="13"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="11"/>
     </row>
-    <row r="5" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="12"/>
-      <c r="F5" s="8">
+    <row r="5" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="10"/>
+      <c r="F5" s="6">
         <v>7</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="5">
+      <c r="G5" s="10">
+        <v>4</v>
+      </c>
+      <c r="H5" s="4">
         <v>3</v>
       </c>
-      <c r="J5" s="8">
-        <v>4</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="N5" s="8">
+      <c r="J5" s="6">
+        <v>4</v>
+      </c>
+      <c r="K5" s="10">
+        <v>2</v>
+      </c>
+      <c r="N5" s="6">
         <v>5</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="12"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="12"/>
+      <c r="O5" s="10"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="10"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="10"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="11">
+        <v>2</v>
+      </c>
       <c r="H6" s="1">
         <v>4</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="9">
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
         <v>3</v>
       </c>
-      <c r="K6" s="13"/>
+      <c r="K6" s="11">
+        <v>2</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="13"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="11">
+        <v>2</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="13"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="11"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="13"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="11"/>
     </row>
-    <row r="7" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="12"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="12"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="5">
+      <c r="B7" s="6"/>
+      <c r="C7" s="10"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="10"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="10">
+        <v>4</v>
+      </c>
+      <c r="L7" s="4">
         <v>3</v>
       </c>
-      <c r="N7" s="8">
-        <v>1</v>
-      </c>
-      <c r="O7" s="12"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="12"/>
-      <c r="V7" s="8">
-        <v>1</v>
-      </c>
-      <c r="W7" s="12"/>
+      <c r="M7" s="4">
+        <v>2</v>
+      </c>
+      <c r="N7" s="6">
+        <v>1</v>
+      </c>
+      <c r="O7" s="10">
+        <v>4</v>
+      </c>
+      <c r="R7" s="6"/>
+      <c r="S7" s="10"/>
+      <c r="V7" s="6">
+        <v>1</v>
+      </c>
+      <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="9">
-        <v>2</v>
-      </c>
-      <c r="G8" s="13"/>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11">
+        <v>2</v>
+      </c>
       <c r="H8" s="1">
         <v>4</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="13"/>
+      <c r="I8" s="16">
+        <v>4</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="11"/>
       <c r="L8" s="1">
         <v>1</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="9">
-        <v>2</v>
-      </c>
-      <c r="O8" s="13"/>
+      <c r="M8" s="16">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
+        <v>2</v>
+      </c>
+      <c r="O8" s="11">
+        <v>2</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="13"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="11"/>
       <c r="T8" s="1">
         <v>1</v>
       </c>
-      <c r="U8" s="1"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="13"/>
+      <c r="U8" s="1">
+        <v>1</v>
+      </c>
+      <c r="V8" s="7">
+        <v>4</v>
+      </c>
+      <c r="W8" s="11">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="10"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="10"/>
+      <c r="I9" s="4">
+        <v>2</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="4">
+        <v>3</v>
+      </c>
+      <c r="M9" s="4">
+        <v>4</v>
+      </c>
+      <c r="N9" s="6">
+        <v>11</v>
+      </c>
+      <c r="O9" s="10">
+        <v>2</v>
+      </c>
+      <c r="R9" s="6"/>
+      <c r="S9" s="10"/>
+      <c r="V9" s="6">
+        <v>1</v>
+      </c>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="12"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="12"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="5">
-        <v>3</v>
-      </c>
-      <c r="N9" s="8">
-        <v>11</v>
-      </c>
-      <c r="O9" s="12"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="12"/>
-      <c r="V9" s="8">
-        <v>1</v>
-      </c>
-      <c r="W9" s="12"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="13"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="13"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="11"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="13"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="11"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="9">
+      <c r="V10" s="7">
         <v>8</v>
       </c>
-      <c r="W10" s="13"/>
+      <c r="W10" s="11">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
@@ -930,6 +981,12 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>